<commit_message>
EXception log and Email added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Nautilus_Prod</t>
+  </si>
+  <si>
+    <t>SendTestMail</t>
+  </si>
+  <si>
+    <t>TestMailTo</t>
+  </si>
+  <si>
+    <t>shibani@digitalalign.com</t>
   </si>
 </sst>
 </file>
@@ -304,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -312,6 +321,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -596,7 +606,7 @@
   <dimension ref="A1:Z951"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -724,9 +734,21 @@
       <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1665,8 +1687,11 @@
     <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2896,7 +2921,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>